<commit_message>
subida de imágenes dia19
</commit_message>
<xml_diff>
--- a/Day19-Dinosaurs/data dinosaurios.xlsx
+++ b/Day19-Dinosaurs/data dinosaurios.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nombre</t>
   </si>
@@ -41,10 +41,16 @@
     <t>Gran dinosaurio carnívoro del período Cretácico en América del Sur. Era uno de los más grandes, alcanzando hasta 13 metros de largo y 8 toneladas de peso.</t>
   </si>
   <si>
-    <t>https://github.com/SergioGerman412/30DayChartChallenge/main/Day18-AsianDevelopmentBank/tasa%20de%20fertilidad.png?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/SergioGerman412/30DayChartChallenge/blob/main/Day17-network/diagrama%20de%20red.png?raw=true</t>
+    <t>https://github.com/SergioGerman412/30DayChartChallenge/blob/main/Day19-Dinosaurs/Im%C3%A1genes/gigantosaurio.png?raw=true</t>
+  </si>
+  <si>
+    <t>https://github.com/SergioGerman412/30DayChartChallenge/blob/main/Day19-Dinosaurs/Imágenes/carcharodontosaurus.jpg?raw=true</t>
+  </si>
+  <si>
+    <t>Carcharodontosaurus</t>
+  </si>
+  <si>
+    <t>Gigantesco terópodo carnívoro que vivió durante el período Cretácico en lo que hoy es África. Se estima que llegaba a medir hasta 13 metros de largo y poseía enormes dientes serrados, similar al Tyrannosaurus rex.</t>
   </si>
 </sst>
 </file>
@@ -376,7 +382,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -409,10 +415,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -421,8 +427,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
subida completa de dia 19
</commit_message>
<xml_diff>
--- a/Day19-Dinosaurs/data dinosaurios.xlsx
+++ b/Day19-Dinosaurs/data dinosaurios.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Nombre</t>
   </si>
@@ -51,6 +51,33 @@
   </si>
   <si>
     <t>Gigantesco terópodo carnívoro que vivió durante el período Cretácico en lo que hoy es África. Se estima que llegaba a medir hasta 13 metros de largo y poseía enormes dientes serrados, similar al Tyrannosaurus rex.</t>
+  </si>
+  <si>
+    <t>Lythronax</t>
+  </si>
+  <si>
+    <t>Mapusaurus</t>
+  </si>
+  <si>
+    <t>Spinosaurus</t>
+  </si>
+  <si>
+    <t>https://github.com/SergioGerman412/30DayChartChallenge/blob/main/Day19-Dinosaurs/Imágenes/lythronax.png?raw=true</t>
+  </si>
+  <si>
+    <t>https://github.com/SergioGerman412/30DayChartChallenge/blob/main/Day19-Dinosaurs/Imágenes/mapusaurus.jpg?raw=true</t>
+  </si>
+  <si>
+    <t>https://github.com/SergioGerman412/30DayChartChallenge/blob/main/Day19-Dinosaurs/Imágenes/spinosaurus.jpg?raw=true</t>
+  </si>
+  <si>
+    <t>Apodado "rey del oeste sangriento", fue un dinosaurio carnívoro que vivió en América del Norte durante el período Cretácico Superior, caracterizado por su gran tamaño y sus afilados dientes serrados.</t>
+  </si>
+  <si>
+    <t>Terópodo gigante que vivió en lo que ahora es Argentina durante el período Cretácico. Conocido por ser uno de los mayores carnívoros que haya existido, este dinosaurio cazaba en manadas y se caracterizaba por su gran tamaño y ferocidad.</t>
+  </si>
+  <si>
+    <t>Habitó en lo que ahora es el norte de África durante el período Cretácico. Es uno de los mayores dinosaurios carnívoros conocidos</t>
   </si>
 </sst>
 </file>
@@ -379,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -424,12 +451,48 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4" display="https://github.com/SergioGerman412/30DayChartChallenge/blob/main/Day19-Dinosaurs/Imágenes/carcharodontosaurus.jpg?raw=true"/>
+    <hyperlink ref="C6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>